<commit_message>
Documentation of Schmitt Trigger inputs
</commit_message>
<xml_diff>
--- a/schematics/kicad/pico-glitcher-v2-extension/production/pico-glitcher-v2.1-extension-BOM.xlsx
+++ b/schematics/kicad/pico-glitcher-v2-extension/production/pico-glitcher-v2.1-extension-BOM.xlsx
@@ -271,13 +271,13 @@
     <t>C103199</t>
   </si>
   <si>
-    <t>500Ω</t>
+    <t>499Ω</t>
   </si>
   <si>
     <t>R19, R22</t>
   </si>
   <si>
-    <t>C860931</t>
+    <t>C23065</t>
   </si>
   <si>
     <t>49.9Ω, 1W</t>

</xml_diff>